<commit_message>
get fucked with these extraction files
</commit_message>
<xml_diff>
--- a/data/extractions/250506 Fiche d'extraction d'échantillons.xlsx
+++ b/data/extractions/250506 Fiche d'extraction d'échantillons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itgitm-my.sharepoint.com/personal/nvanreet_itg_be/Documents/Documenten/GitHub/biobank-dashboard/data/extractions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D09A5C61-EC37-45A5-8232-4EE57BC924C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E8488CB-DCAB-446E-9409-EF1772BC0896}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{D09A5C61-EC37-45A5-8232-4EE57BC924C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46867EFC-9E53-4D8E-892E-BEE9FF5CDEA0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1CE68EB6-DB45-45E9-95B2-F2EDACD56A3B}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Extractions!$A$1:$L$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Extractions!$A$1:$L$65</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Extractions!$A$1:$L$11</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Extractions!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -337,6 +337,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -638,9 +642,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F8F8353-8CB1-400B-B8E5-1BA03F155009}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,26 +1089,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Uploaded xmlns="974e1998-2087-4290-81d3-cf83f1cc5cbf">2025-05-08T09:38:06+00:00</Uploaded>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="974e1998-2087-4290-81d3-cf83f1cc5cbf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005F56A3FBA1F9FF429D4C886089ACEF10" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="93e6b79bffcb710984822118ae45b29f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="974e1998-2087-4290-81d3-cf83f1cc5cbf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c971e98cb6cdb6e05177eaad282d8065" ns2:_="">
     <xsd:import namespace="974e1998-2087-4290-81d3-cf83f1cc5cbf"/>
@@ -1282,25 +1266,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5842555D-F7D5-4D17-B1E8-F881B15C9E16}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="974e1998-2087-4290-81d3-cf83f1cc5cbf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ED371F3-D97D-417E-BCDD-221E96D58658}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Uploaded xmlns="974e1998-2087-4290-81d3-cf83f1cc5cbf">2025-05-08T09:38:06+00:00</Uploaded>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="974e1998-2087-4290-81d3-cf83f1cc5cbf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4C432F4-32BA-4FF8-A5EC-5A6911D0D5A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1316,4 +1302,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ED371F3-D97D-417E-BCDD-221E96D58658}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5842555D-F7D5-4D17-B1E8-F881B15C9E16}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="974e1998-2087-4290-81d3-cf83f1cc5cbf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>